<commit_message>
updated code for 2015
</commit_message>
<xml_diff>
--- a/data/03 application country numbers per year.xlsx
+++ b/data/03 application country numbers per year.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>project_year</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,15 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>428</v>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>